<commit_message>
update assessent output style
</commit_message>
<xml_diff>
--- a/assessment/考核模版.xlsx
+++ b/assessment/考核模版.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15060" activeTab="1"/>
+    <workbookView windowWidth="23400" windowHeight="23960" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="要求" sheetId="3" r:id="rId1"/>
@@ -427,17 +427,11 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Regular"/>
-        <charset val="134"/>
-      </rPr>
       <t>A</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
@@ -447,17 +441,11 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Regular"/>
-        <charset val="134"/>
-      </rPr>
       <t>B</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
@@ -485,7 +473,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,38 +489,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="黑体"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Regular"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial Regular"/>
       <charset val="134"/>
@@ -541,6 +530,12 @@
       <sz val="9.75"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1056,137 +1051,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1211,43 +1206,55 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1584,46 +1591,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="112.875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="112.875" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1639,7 +1646,7 @@
   <sheetPr/>
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
@@ -1653,1060 +1660,1060 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="21" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="7" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="21"/>
+      <c r="E9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="7" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="22" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="21"/>
+      <c r="D17" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="7" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="7" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="7" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="7" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7" t="s">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="7" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8" t="s">
+      <c r="D32" s="21"/>
+      <c r="E32" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="7" t="s">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="7" t="s">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8" t="s">
+      <c r="D35" s="21"/>
+      <c r="E35" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7" t="s">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="7" t="s">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8" t="s">
+      <c r="D38" s="21"/>
+      <c r="E38" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="23" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="7" t="s">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="22" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8" t="s">
+      <c r="D40" s="21"/>
+      <c r="E40" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="22" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="7" t="s">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="22" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7" t="s">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="22" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8" t="s">
+      <c r="D43" s="21"/>
+      <c r="E43" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="22" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="7" t="s">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="22" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8" t="s">
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="22" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="7" t="s">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7" t="s">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="22" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="7" t="s">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="22" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="20" t="s">
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="24" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="7" t="s">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="7" t="s">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="7" t="s">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="7" t="s">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="22" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="7" t="s">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="7" t="s">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="22" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="7" t="s">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="22" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="7" t="s">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8" t="s">
+      <c r="B58" s="21"/>
+      <c r="C58" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8" t="s">
+      <c r="D58" s="21"/>
+      <c r="E58" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F58" s="22" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="7" t="s">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="22" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="7" t="s">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="20" t="s">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="7" t="s">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="22" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="7" t="s">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="22" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="7" t="s">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="22" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="7" t="s">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="22" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="7" t="s">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="22" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="7" t="s">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="22" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="7" t="s">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="22" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8" t="s">
+      <c r="B69" s="21"/>
+      <c r="C69" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8" t="s">
+      <c r="D69" s="21"/>
+      <c r="E69" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="F69" s="22" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="7" t="s">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="7" t="s">
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="22" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="8"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="20" t="s">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="24" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="7" t="s">
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="7" t="s">
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="22" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="8"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="7" t="s">
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="22" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="7" t="s">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="7" t="s">
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="22" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="7" t="s">
+      <c r="A78" s="21"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="22" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="7" t="s">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="22" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="8"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="7" t="s">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="22" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8" t="s">
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="F81" s="6" t="s">
+      <c r="F81" s="23" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="7" t="s">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="22" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="7" t="s">
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="22" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="7" t="s">
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="7" t="s">
+      <c r="A85" s="21"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="22" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="7" t="s">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="8"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="7" t="s">
+      <c r="A87" s="21"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="22" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="8"/>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="7" t="s">
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="22" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="8"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="7" t="s">
+      <c r="A89" s="21"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="22" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="8"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="7" t="s">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="22" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="8"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="7" t="s">
+      <c r="A91" s="21"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="22" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="8"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="7" t="s">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="22" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="8"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="7" t="s">
+      <c r="A93" s="21"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="22" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="8"/>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="7" t="s">
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="22" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2913,310 +2920,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="20">
         <v>0.1</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="20">
         <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="20">
         <v>0.1</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="20">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="20">
         <v>0.1</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="20">
         <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="20">
         <v>0.1</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="20">
         <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="20">
         <v>0.1</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="20">
         <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="20">
         <v>0.2</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="20">
         <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="20">
         <v>0.2</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="20">
         <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="20">
         <v>0.2</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="20">
         <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="20">
         <v>0.2</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="20">
         <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="20">
         <v>0.2</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="20">
         <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="20">
         <v>0.3</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="20">
         <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="20">
         <v>0.3</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="20">
         <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="20">
         <v>0.3</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="20">
         <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="20">
         <v>0.3</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="20">
         <v>0.9</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="20">
         <v>0.3</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="20">
         <v>0.9</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="20">
         <v>0.5</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="20">
         <v>0.5</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="20">
         <v>0.5</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="20">
         <v>0.5</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="20">
         <v>0.5</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="20">
         <v>0.5</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="20">
         <v>0</v>
       </c>
     </row>
@@ -3231,16 +3238,15 @@
   <sheetPr/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="7.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="26.9285714285714" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.2857142857143" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="47" customHeight="1" spans="1:4">
@@ -3251,7 +3257,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:4">
+    <row r="2" ht="17" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
         <v>125</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:4">
+    <row r="3" ht="17" customHeight="1" spans="1:4">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3277,7 +3283,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:4">
+    <row r="4" ht="17" customHeight="1" spans="1:4">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -3289,7 +3295,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:4">
+    <row r="5" ht="17" customHeight="1" spans="1:4">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -3301,7 +3307,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:4">
+    <row r="6" ht="17" customHeight="1" spans="1:4">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -3313,7 +3319,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:4">
+    <row r="7" ht="17" customHeight="1" spans="1:4">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -3325,7 +3331,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:4">
+    <row r="8" ht="17" customHeight="1" spans="1:4">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -3337,7 +3343,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:4">
+    <row r="9" ht="17" customHeight="1" spans="1:4">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -3349,7 +3355,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:4">
+    <row r="10" ht="17" customHeight="1" spans="1:4">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3361,7 +3367,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="1:4">
+    <row r="11" ht="17" customHeight="1" spans="1:4">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3373,7 +3379,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:4">
+    <row r="12" ht="17" customHeight="1" spans="1:4">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3385,7 +3391,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="1:4">
+    <row r="13" ht="17" customHeight="1" spans="1:4">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3397,7 +3403,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:4">
+    <row r="14" ht="17" customHeight="1" spans="1:4">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -3409,13 +3415,13 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" ht="35" customHeight="1" spans="1:4">
+    <row r="15" ht="41" customHeight="1" spans="1:4">
       <c r="A15" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16"/>
@@ -3423,67 +3429,67 @@
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" ht="17" spans="1:4">
-      <c r="A17" s="10" t="s">
+    <row r="17" ht="18" spans="1:4">
+      <c r="A17" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="12">
         <v>12</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" ht="17" spans="1:4">
-      <c r="A18" s="10" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" ht="18" spans="1:4">
+      <c r="A18" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="14" t="s">
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" ht="17.6" spans="1:4">
+      <c r="A19" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="16">
         <v>0.2</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="16">
         <v>0.4</v>
       </c>
-      <c r="D19" s="16"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="14" t="s">
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" ht="17.6" spans="1:4">
+      <c r="A20" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="16">
         <f>B17*0.3+B19</f>
         <v>3.8</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="16">
         <f>B17*0.4+C19</f>
         <v>5.2</v>
       </c>
-      <c r="D20" s="16"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="14" t="s">
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" ht="17.6" spans="1:4">
+      <c r="A21" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="18">
         <f>B20-INT(B20)</f>
         <v>0.8</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="18">
         <f>C20-INT(C20)</f>
         <v>0.200000000000001</v>
       </c>
-      <c r="D21" s="18"/>
+      <c r="D21" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>